<commit_message>
New branch with chrome added properties
</commit_message>
<xml_diff>
--- a/OutputFiles/TC01_Canine_Filter_Breed-Akita_Neo4jData.xlsx
+++ b/OutputFiles/TC01_Canine_Filter_Breed-Akita_Neo4jData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="36">
   <si>
     <t>Case ID</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Akita']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+  </si>
+  <si>
+    <t>C:\Katalon_mastercopy520\DataCommons_Automation\OutputFiles\TC01_Canine_Filter_Breed-Akita_Neo4jData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +712,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -759,7 +762,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated canine keywords; added samples, files obj
</commit_message>
<xml_diff>
--- a/OutputFiles/TC01_Canine_Filter_Breed-Akita_Neo4jData.xlsx
+++ b/OutputFiles/TC01_Canine_Filter_Breed-Akita_Neo4jData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="39">
   <si>
     <t>Case ID</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Cypher query should not be an empty string</t>
+  </si>
+  <si>
+    <t>NCATS-COP01-CCB010072</t>
+  </si>
+  <si>
+    <t>Osteosarcoma</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -219,10 +228,10 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>

</xml_diff>